<commit_message>
Few more bug fixes
</commit_message>
<xml_diff>
--- a/gui/angles_smooth_changed.xlsx
+++ b/gui/angles_smooth_changed.xlsx
@@ -884,8 +884,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M499"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A178" workbookViewId="0">
-      <selection activeCell="D210" sqref="D210"/>
+    <sheetView tabSelected="1" topLeftCell="A230" workbookViewId="0">
+      <selection activeCell="D259" sqref="D259"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9470,7 +9470,7 @@
         <v>1</v>
       </c>
       <c r="D210">
-        <v>12.5</v>
+        <v>13.5</v>
       </c>
       <c r="E210">
         <v>62.9</v>
@@ -9552,7 +9552,7 @@
         <v>3</v>
       </c>
       <c r="D212">
-        <v>19</v>
+        <v>18.5</v>
       </c>
       <c r="E212">
         <v>64</v>
@@ -9839,7 +9839,7 @@
         <v>10</v>
       </c>
       <c r="D219">
-        <v>38</v>
+        <v>38.5</v>
       </c>
       <c r="E219">
         <v>67.099999999999994</v>
@@ -9880,7 +9880,7 @@
         <v>11</v>
       </c>
       <c r="D220">
-        <v>41</v>
+        <v>41.5</v>
       </c>
       <c r="E220">
         <v>67.5</v>
@@ -9921,7 +9921,7 @@
         <v>12</v>
       </c>
       <c r="D221">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E221">
         <v>67.900000000000006</v>
@@ -9962,7 +9962,7 @@
         <v>13</v>
       </c>
       <c r="D222">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E222">
         <v>68.400000000000006</v>
@@ -10003,7 +10003,7 @@
         <v>14</v>
       </c>
       <c r="D223">
-        <v>50</v>
+        <v>50.5</v>
       </c>
       <c r="E223">
         <v>69</v>
@@ -10044,7 +10044,7 @@
         <v>15</v>
       </c>
       <c r="D224">
-        <v>52</v>
+        <v>52.5</v>
       </c>
       <c r="E224">
         <v>69.3</v>
@@ -10085,7 +10085,7 @@
         <v>16</v>
       </c>
       <c r="D225">
-        <v>54</v>
+        <v>55.5</v>
       </c>
       <c r="E225">
         <v>69.5</v>
@@ -10126,7 +10126,7 @@
         <v>17</v>
       </c>
       <c r="D226">
-        <v>57.5</v>
+        <v>58.5</v>
       </c>
       <c r="E226">
         <v>69.900000000000006</v>
@@ -10167,7 +10167,7 @@
         <v>18</v>
       </c>
       <c r="D227">
-        <v>60</v>
+        <v>61.5</v>
       </c>
       <c r="E227">
         <v>70.099999999999994</v>
@@ -10208,7 +10208,7 @@
         <v>19</v>
       </c>
       <c r="D228">
-        <v>62.5</v>
+        <v>64.5</v>
       </c>
       <c r="E228">
         <v>70.3</v>
@@ -10249,7 +10249,7 @@
         <v>20</v>
       </c>
       <c r="D229">
-        <v>65.5</v>
+        <v>66.5</v>
       </c>
       <c r="E229">
         <v>70.7</v>
@@ -10290,7 +10290,7 @@
         <v>21</v>
       </c>
       <c r="D230">
-        <v>68.5</v>
+        <v>69.5</v>
       </c>
       <c r="E230">
         <v>71</v>
@@ -10331,7 +10331,7 @@
         <v>22</v>
       </c>
       <c r="D231">
-        <v>71</v>
+        <v>71.5</v>
       </c>
       <c r="E231">
         <v>70.7</v>
@@ -10372,7 +10372,7 @@
         <v>23</v>
       </c>
       <c r="D232">
-        <v>77</v>
+        <v>75.5</v>
       </c>
       <c r="E232">
         <v>68.400000000000006</v>
@@ -10413,7 +10413,7 @@
         <v>24</v>
       </c>
       <c r="D233">
-        <v>79.5</v>
+        <v>78.5</v>
       </c>
       <c r="E233">
         <v>67.900000000000006</v>
@@ -10454,7 +10454,7 @@
         <v>25</v>
       </c>
       <c r="D234">
-        <v>82</v>
+        <v>81.5</v>
       </c>
       <c r="E234">
         <v>67.3</v>
@@ -10495,7 +10495,7 @@
         <v>1</v>
       </c>
       <c r="D235">
-        <v>12.5</v>
+        <v>14.5</v>
       </c>
       <c r="E235">
         <v>62.9</v>
@@ -10536,7 +10536,7 @@
         <v>2</v>
       </c>
       <c r="D236">
-        <v>15.5</v>
+        <v>17.5</v>
       </c>
       <c r="E236">
         <v>63.5</v>
@@ -10577,7 +10577,7 @@
         <v>3</v>
       </c>
       <c r="D237">
-        <v>19</v>
+        <v>20.5</v>
       </c>
       <c r="E237">
         <v>64</v>
@@ -10618,7 +10618,7 @@
         <v>4</v>
       </c>
       <c r="D238">
-        <v>21.5</v>
+        <v>23.5</v>
       </c>
       <c r="E238">
         <v>64.5</v>
@@ -10659,7 +10659,7 @@
         <v>5</v>
       </c>
       <c r="D239">
-        <v>24.5</v>
+        <v>26</v>
       </c>
       <c r="E239">
         <v>65</v>
@@ -10700,7 +10700,7 @@
         <v>6</v>
       </c>
       <c r="D240">
-        <v>27.5</v>
+        <v>29</v>
       </c>
       <c r="E240">
         <v>65.2</v>
@@ -10741,7 +10741,7 @@
         <v>7</v>
       </c>
       <c r="D241">
-        <v>30</v>
+        <v>32.5</v>
       </c>
       <c r="E241">
         <v>66.5</v>
@@ -10782,7 +10782,7 @@
         <v>8</v>
       </c>
       <c r="D242">
-        <v>32.5</v>
+        <v>35</v>
       </c>
       <c r="E242">
         <v>66.099999999999994</v>
@@ -10823,7 +10823,7 @@
         <v>9</v>
       </c>
       <c r="D243">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E243">
         <v>66.599999999999994</v>
@@ -10864,7 +10864,7 @@
         <v>10</v>
       </c>
       <c r="D244">
-        <v>38</v>
+        <v>40.5</v>
       </c>
       <c r="E244">
         <v>67.099999999999994</v>
@@ -10905,7 +10905,7 @@
         <v>11</v>
       </c>
       <c r="D245">
-        <v>41</v>
+        <v>43.5</v>
       </c>
       <c r="E245">
         <v>67.5</v>
@@ -10946,7 +10946,7 @@
         <v>12</v>
       </c>
       <c r="D246">
-        <v>44</v>
+        <v>46.5</v>
       </c>
       <c r="E246">
         <v>67.900000000000006</v>
@@ -10987,7 +10987,7 @@
         <v>13</v>
       </c>
       <c r="D247">
-        <v>47</v>
+        <v>49.5</v>
       </c>
       <c r="E247">
         <v>68.400000000000006</v>
@@ -11028,7 +11028,7 @@
         <v>14</v>
       </c>
       <c r="D248">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="E248">
         <v>69</v>
@@ -11069,7 +11069,7 @@
         <v>15</v>
       </c>
       <c r="D249">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="E249">
         <v>69.3</v>
@@ -11110,7 +11110,7 @@
         <v>16</v>
       </c>
       <c r="D250">
-        <v>54</v>
+        <v>57.5</v>
       </c>
       <c r="E250">
         <v>69.5</v>
@@ -11151,7 +11151,7 @@
         <v>17</v>
       </c>
       <c r="D251">
-        <v>57.5</v>
+        <v>60.5</v>
       </c>
       <c r="E251">
         <v>69.900000000000006</v>
@@ -11192,7 +11192,7 @@
         <v>18</v>
       </c>
       <c r="D252">
-        <v>60</v>
+        <v>63.5</v>
       </c>
       <c r="E252">
         <v>70.099999999999994</v>
@@ -11233,7 +11233,7 @@
         <v>19</v>
       </c>
       <c r="D253">
-        <v>62.5</v>
+        <v>66</v>
       </c>
       <c r="E253">
         <v>70.3</v>
@@ -11274,7 +11274,7 @@
         <v>20</v>
       </c>
       <c r="D254">
-        <v>65.5</v>
+        <v>68.5</v>
       </c>
       <c r="E254">
         <v>70.7</v>
@@ -11315,7 +11315,7 @@
         <v>21</v>
       </c>
       <c r="D255">
-        <v>68.5</v>
+        <v>71</v>
       </c>
       <c r="E255">
         <v>71</v>
@@ -11356,7 +11356,7 @@
         <v>22</v>
       </c>
       <c r="D256">
-        <v>71</v>
+        <v>73.5</v>
       </c>
       <c r="E256">
         <v>70.7</v>
@@ -11397,7 +11397,7 @@
         <v>23</v>
       </c>
       <c r="D257">
-        <v>77.5</v>
+        <v>77</v>
       </c>
       <c r="E257">
         <v>68.400000000000006</v>

</xml_diff>